<commit_message>
introduced  keypad into X2A
</commit_message>
<xml_diff>
--- a/size.xlsx
+++ b/size.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>#of char</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>size 2</t>
-  </si>
-  <si>
-    <t>cc</t>
   </si>
   <si>
     <t>receive</t>
@@ -388,7 +385,7 @@
   <dimension ref="D3:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,7 +404,7 @@
     </row>
     <row r="5" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D5" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -417,9 +414,7 @@
       </c>
     </row>
     <row r="6" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="4:12" x14ac:dyDescent="0.25">
@@ -434,17 +429,17 @@
         <v>5</v>
       </c>
       <c r="L8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D9" s="1">
         <f>(128-((D5*5)+(D5-E5)))/2</f>
-        <v>31.5</v>
+        <v>28.5</v>
       </c>
       <c r="E9" s="1">
         <f>(128-((D5*10)+(D5-E5)))/2</f>
-        <v>4</v>
+        <v>-1.5</v>
       </c>
     </row>
     <row r="10" spans="4:12" x14ac:dyDescent="0.25">

</xml_diff>